<commit_message>
added one missed link
</commit_message>
<xml_diff>
--- a/landlibrary/importers/Rural21/20170223 - Rural21 - Land Library Metadata_EN_1-4.xlsx
+++ b/landlibrary/importers/Rural21/20170223 - Rural21 - Land Library Metadata_EN_1-4.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Rural21 - Land Library Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="20170223 - Rural21 - Land Libra" sheetId="1" r:id="rId1"/>
     <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1123" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="569">
   <si>
     <t>Abstract/Description</t>
   </si>
@@ -1530,15 +1530,6 @@
     <t>Michèle Stark</t>
   </si>
   <si>
-    <t>Rebecca Metzner; 
-Nicole Franz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food and Agriculture Organization
-of the United Nations (FAO)
-</t>
-  </si>
-  <si>
     <t>Mecki Kronen;
 Arnoud Meijberg;
 Ines Reinhard</t>
@@ -1876,6 +1867,15 @@
   </si>
   <si>
     <t>sustainable development; land investments; development agencies; research; farming systems; rural development; local community; rural population</t>
+  </si>
+  <si>
+    <t>http://www.rural21.com/uploads/media/rural2014_01-S12-15.pdf</t>
+  </si>
+  <si>
+    <t>Food and Agriculture Organization of the United Nations (FAO)</t>
+  </si>
+  <si>
+    <t>Rebecca Metzner;  Nicole Franz</t>
   </si>
 </sst>
 </file>
@@ -2306,9 +2306,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2343,7 +2343,7 @@
         <v>42</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
@@ -2352,16 +2352,16 @@
         <v>0</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>483</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>484</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>485</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>486</v>
-      </c>
       <c r="I1" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>7</v>
@@ -2373,16 +2373,16 @@
         <v>10</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>18</v>
@@ -2391,7 +2391,7 @@
         <v>6</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>14</v>
@@ -2405,7 +2405,7 @@
         <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>43</v>
@@ -2420,7 +2420,7 @@
         <v>442</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>40</v>
@@ -2448,7 +2448,7 @@
         <v>72</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="7" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
@@ -2459,7 +2459,7 @@
         <v>36</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>49</v>
@@ -2472,7 +2472,7 @@
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>40</v>
@@ -2484,7 +2484,7 @@
         <v>9</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="N3" s="8" t="s">
         <v>364</v>
@@ -2505,7 +2505,7 @@
         <v>208</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="7" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
@@ -2516,7 +2516,7 @@
         <v>36</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>54</v>
@@ -2531,7 +2531,7 @@
         <v>443</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>40</v>
@@ -2543,7 +2543,7 @@
         <v>9</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>366</v>
@@ -2567,7 +2567,7 @@
         <v>124</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="7" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
@@ -2578,7 +2578,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>58</v>
@@ -2590,10 +2590,10 @@
         <v>88</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I5" s="8" t="s">
         <v>40</v>
@@ -2627,7 +2627,7 @@
         <v>125</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="7" customFormat="1" ht="93.6" x14ac:dyDescent="0.3">
@@ -2638,7 +2638,7 @@
         <v>36</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>59</v>
@@ -2653,7 +2653,7 @@
         <v>444</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>40</v>
@@ -2665,10 +2665,10 @@
         <v>9</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="N6" s="8" t="s">
         <v>367</v>
@@ -2687,7 +2687,7 @@
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="7" customFormat="1" ht="109.2" x14ac:dyDescent="0.3">
@@ -2698,7 +2698,7 @@
         <v>36</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>60</v>
@@ -2710,10 +2710,10 @@
         <v>94</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>40</v>
@@ -2725,7 +2725,7 @@
         <v>9</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>373</v>
@@ -2749,7 +2749,7 @@
         <v>126</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="103.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2760,7 +2760,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>37</v>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>40</v>
@@ -2809,7 +2809,7 @@
         <v>128</v>
       </c>
       <c r="T8" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
@@ -2822,7 +2822,7 @@
         <v>36</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>61</v>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>40</v>
@@ -2871,7 +2871,7 @@
         <v>127</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="171.6" x14ac:dyDescent="0.3">
@@ -2882,7 +2882,7 @@
         <v>36</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>62</v>
@@ -2892,10 +2892,10 @@
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>40</v>
@@ -2931,7 +2931,7 @@
         <v>129</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:22" ht="62.4" x14ac:dyDescent="0.3">
@@ -2942,7 +2942,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>63</v>
@@ -2954,10 +2954,10 @@
         <v>102</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>40</v>
@@ -2975,7 +2975,7 @@
         <v>385</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O11" s="8" t="s">
         <v>383</v>
@@ -2993,7 +2993,7 @@
         <v>130</v>
       </c>
       <c r="T11" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="12" spans="1:22" ht="93.6" x14ac:dyDescent="0.3">
@@ -3004,7 +3004,7 @@
         <v>36</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>64</v>
@@ -3017,7 +3017,7 @@
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>40</v>
@@ -3029,7 +3029,7 @@
         <v>9</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>386</v>
@@ -3053,7 +3053,7 @@
         <v>131</v>
       </c>
       <c r="T12" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="93.6" x14ac:dyDescent="0.3">
@@ -3064,7 +3064,7 @@
         <v>36</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>65</v>
@@ -3077,7 +3077,7 @@
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>40</v>
@@ -3089,7 +3089,7 @@
         <v>9</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="M13" s="8" t="s">
         <v>387</v>
@@ -3113,7 +3113,7 @@
         <v>132</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="93.6" x14ac:dyDescent="0.3">
@@ -3124,7 +3124,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>66</v>
@@ -3136,10 +3136,10 @@
         <v>108</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>40</v>
@@ -3175,7 +3175,7 @@
         <v>133</v>
       </c>
       <c r="T14" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="109.2" x14ac:dyDescent="0.3">
@@ -3186,7 +3186,7 @@
         <v>36</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>67</v>
@@ -3199,7 +3199,7 @@
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>40</v>
@@ -3235,7 +3235,7 @@
         <v>134</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="124.8" x14ac:dyDescent="0.3">
@@ -3246,7 +3246,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>68</v>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>40</v>
@@ -3277,7 +3277,7 @@
         <v>377</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O16" s="8" t="s">
         <v>365</v>
@@ -3295,7 +3295,7 @@
         <v>135</v>
       </c>
       <c r="T16" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="207" customHeight="1" x14ac:dyDescent="0.3">
@@ -3306,7 +3306,7 @@
         <v>36</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>69</v>
@@ -3319,7 +3319,7 @@
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>40</v>
@@ -3334,10 +3334,10 @@
         <v>391</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O17" s="8" t="s">
         <v>392</v>
@@ -3355,7 +3355,7 @@
         <v>136</v>
       </c>
       <c r="T17" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -3366,7 +3366,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>70</v>
@@ -3379,7 +3379,7 @@
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>40</v>
@@ -3413,7 +3413,7 @@
         <v>137</v>
       </c>
       <c r="T18" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -3424,7 +3424,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>71</v>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>40</v>
@@ -3471,7 +3471,7 @@
         <v>138</v>
       </c>
       <c r="T19" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -3482,7 +3482,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>142</v>
@@ -3494,10 +3494,10 @@
         <v>446</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>40</v>
@@ -3530,7 +3530,7 @@
         <v>158</v>
       </c>
       <c r="T20" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="21" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -3541,7 +3541,7 @@
         <v>141</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>143</v>
@@ -3556,7 +3556,7 @@
         <v>443</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>40</v>
@@ -3568,7 +3568,7 @@
         <v>9</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>398</v>
@@ -3589,7 +3589,7 @@
         <v>162</v>
       </c>
       <c r="T21" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="140.4" x14ac:dyDescent="0.3">
@@ -3600,7 +3600,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D22" s="11" t="s">
         <v>144</v>
@@ -3612,10 +3612,10 @@
         <v>207</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>40</v>
@@ -3633,7 +3633,7 @@
         <v>366</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>365</v>
@@ -3651,7 +3651,7 @@
         <v>166</v>
       </c>
       <c r="T22" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="140.4" x14ac:dyDescent="0.3">
@@ -3662,7 +3662,7 @@
         <v>141</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>145</v>
@@ -3675,7 +3675,7 @@
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>40</v>
@@ -3687,7 +3687,7 @@
         <v>9</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>366</v>
@@ -3708,7 +3708,7 @@
         <v>170</v>
       </c>
       <c r="T23" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -3719,7 +3719,7 @@
         <v>141</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D24" s="11" t="s">
         <v>146</v>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>40</v>
@@ -3765,7 +3765,7 @@
         <v>175</v>
       </c>
       <c r="T24" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -3776,7 +3776,7 @@
         <v>141</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>147</v>
@@ -3791,7 +3791,7 @@
         <v>443</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>40</v>
@@ -3824,7 +3824,7 @@
         <v>179</v>
       </c>
       <c r="T25" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -3835,7 +3835,7 @@
         <v>141</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D26" s="11" t="s">
         <v>148</v>
@@ -3848,7 +3848,7 @@
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>40</v>
@@ -3881,7 +3881,7 @@
         <v>209</v>
       </c>
       <c r="T26" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -3892,7 +3892,7 @@
         <v>141</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>149</v>
@@ -3905,7 +3905,7 @@
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>40</v>
@@ -3920,7 +3920,7 @@
         <v>403</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>365</v>
@@ -3938,7 +3938,7 @@
         <v>186</v>
       </c>
       <c r="T27" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -3949,7 +3949,7 @@
         <v>141</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>150</v>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>40</v>
@@ -3977,7 +3977,7 @@
         <v>404</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>365</v>
@@ -3995,7 +3995,7 @@
         <v>189</v>
       </c>
       <c r="T28" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -4006,7 +4006,7 @@
         <v>141</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>151</v>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>40</v>
@@ -4037,7 +4037,7 @@
         <v>366</v>
       </c>
       <c r="N29" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>406</v>
@@ -4055,7 +4055,7 @@
         <v>194</v>
       </c>
       <c r="T29" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="156" x14ac:dyDescent="0.3">
@@ -4066,7 +4066,7 @@
         <v>141</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>152</v>
@@ -4078,10 +4078,10 @@
         <v>196</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>40</v>
@@ -4099,7 +4099,7 @@
         <v>366</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>408</v>
@@ -4117,7 +4117,7 @@
         <v>199</v>
       </c>
       <c r="T30" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="156" x14ac:dyDescent="0.3">
@@ -4128,7 +4128,7 @@
         <v>141</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>153</v>
@@ -4140,10 +4140,10 @@
         <v>201</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>40</v>
@@ -4161,7 +4161,7 @@
         <v>366</v>
       </c>
       <c r="N31" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>374</v>
@@ -4179,7 +4179,7 @@
         <v>189</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="140.4" x14ac:dyDescent="0.3">
@@ -4190,7 +4190,7 @@
         <v>211</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>226</v>
@@ -4205,7 +4205,7 @@
         <v>443</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>40</v>
@@ -4223,7 +4223,7 @@
         <v>398</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O32" s="8" t="s">
         <v>365</v>
@@ -4241,7 +4241,7 @@
         <v>230</v>
       </c>
       <c r="T32" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -4252,7 +4252,7 @@
         <v>211</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>212</v>
@@ -4267,7 +4267,7 @@
         <v>443</v>
       </c>
       <c r="H33" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>40</v>
@@ -4283,7 +4283,7 @@
       </c>
       <c r="M33" s="8"/>
       <c r="N33" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O33" s="8" t="s">
         <v>365</v>
@@ -4301,7 +4301,7 @@
         <v>235</v>
       </c>
       <c r="T33" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -4312,7 +4312,7 @@
         <v>211</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>213</v>
@@ -4327,7 +4327,7 @@
         <v>443</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>40</v>
@@ -4345,7 +4345,7 @@
         <v>377</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O34" s="8" t="s">
         <v>365</v>
@@ -4363,7 +4363,7 @@
         <v>240</v>
       </c>
       <c r="T34" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -4374,7 +4374,7 @@
         <v>211</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>214</v>
@@ -4387,7 +4387,7 @@
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>40</v>
@@ -4403,7 +4403,7 @@
       </c>
       <c r="M35" s="8"/>
       <c r="N35" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O35" s="8" t="s">
         <v>365</v>
@@ -4421,7 +4421,7 @@
         <v>245</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -4432,7 +4432,7 @@
         <v>211</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D36" s="11" t="s">
         <v>215</v>
@@ -4441,10 +4441,10 @@
         <v>246</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>40</v>
@@ -4460,7 +4460,7 @@
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O36" s="8" t="s">
         <v>365</v>
@@ -4478,7 +4478,7 @@
         <v>249</v>
       </c>
       <c r="T36" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -4489,7 +4489,7 @@
         <v>211</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D37" s="11" t="s">
         <v>216</v>
@@ -4502,7 +4502,7 @@
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>40</v>
@@ -4518,7 +4518,7 @@
       </c>
       <c r="M37" s="8"/>
       <c r="N37" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O37" s="8" t="s">
         <v>365</v>
@@ -4536,7 +4536,7 @@
         <v>253</v>
       </c>
       <c r="T37" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="38" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -4547,7 +4547,7 @@
         <v>211</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>217</v>
@@ -4556,13 +4556,13 @@
         <v>254</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>455</v>
+        <v>568</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>456</v>
+        <v>567</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>40</v>
@@ -4580,7 +4580,7 @@
         <v>366</v>
       </c>
       <c r="N38" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O38" s="8" t="s">
         <v>365</v>
@@ -4598,7 +4598,7 @@
         <v>257</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -4609,7 +4609,7 @@
         <v>211</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>218</v>
@@ -4622,7 +4622,7 @@
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>40</v>
@@ -4634,13 +4634,13 @@
         <v>9</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>366</v>
       </c>
       <c r="N39" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O39" s="8" t="s">
         <v>396</v>
@@ -4658,7 +4658,7 @@
         <v>262</v>
       </c>
       <c r="T39" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -4669,7 +4669,7 @@
         <v>211</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D40" s="11" t="s">
         <v>219</v>
@@ -4678,13 +4678,13 @@
         <v>263</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>443</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>40</v>
@@ -4702,7 +4702,7 @@
         <v>418</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O40" s="8" t="s">
         <v>406</v>
@@ -4720,7 +4720,7 @@
         <v>266</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -4731,7 +4731,7 @@
         <v>211</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D41" s="11" t="s">
         <v>220</v>
@@ -4740,11 +4740,11 @@
         <v>267</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>40</v>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="M41" s="8"/>
       <c r="N41" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O41" s="8" t="s">
         <v>420</v>
@@ -4778,7 +4778,7 @@
         <v>270</v>
       </c>
       <c r="T41" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="156" x14ac:dyDescent="0.3">
@@ -4789,7 +4789,7 @@
         <v>211</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D42" s="11" t="s">
         <v>221</v>
@@ -4798,13 +4798,13 @@
         <v>271</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>40</v>
@@ -4822,7 +4822,7 @@
         <v>421</v>
       </c>
       <c r="N42" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O42" s="8" t="s">
         <v>422</v>
@@ -4840,7 +4840,7 @@
         <v>274</v>
       </c>
       <c r="T42" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="43" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -4851,7 +4851,7 @@
         <v>211</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D43" s="11" t="s">
         <v>222</v>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>40</v>
@@ -4882,7 +4882,7 @@
         <v>377</v>
       </c>
       <c r="N43" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O43" s="8" t="s">
         <v>365</v>
@@ -4900,7 +4900,7 @@
         <v>279</v>
       </c>
       <c r="T43" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="44" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -4911,7 +4911,7 @@
         <v>211</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D44" s="11" t="s">
         <v>223</v>
@@ -4923,10 +4923,10 @@
         <v>281</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>40</v>
@@ -4944,7 +4944,7 @@
         <v>377</v>
       </c>
       <c r="N44" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O44" s="8" t="s">
         <v>365</v>
@@ -4962,7 +4962,7 @@
         <v>284</v>
       </c>
       <c r="T44" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="45" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -4973,7 +4973,7 @@
         <v>211</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>224</v>
@@ -4986,7 +4986,7 @@
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>40</v>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="M45" s="8"/>
       <c r="N45" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O45" s="8" t="s">
         <v>427</v>
@@ -5020,7 +5020,7 @@
         <v>289</v>
       </c>
       <c r="T45" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="46" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -5031,7 +5031,7 @@
         <v>211</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>225</v>
@@ -5040,11 +5040,11 @@
         <v>290</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>40</v>
@@ -5060,7 +5060,7 @@
       </c>
       <c r="M46" s="8"/>
       <c r="N46" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O46" s="8" t="s">
         <v>371</v>
@@ -5078,7 +5078,7 @@
         <v>293</v>
       </c>
       <c r="T46" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="47" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -5089,7 +5089,7 @@
         <v>295</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>296</v>
@@ -5098,13 +5098,13 @@
         <v>309</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G47" s="8" t="s">
         <v>443</v>
       </c>
       <c r="H47" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>40</v>
@@ -5122,7 +5122,7 @@
         <v>366</v>
       </c>
       <c r="N47" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O47" s="1" t="s">
         <v>365</v>
@@ -5140,7 +5140,7 @@
         <v>312</v>
       </c>
       <c r="T47" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="48" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -5151,7 +5151,7 @@
         <v>295</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="D48" s="11" t="s">
         <v>297</v>
@@ -5164,7 +5164,7 @@
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>40</v>
@@ -5182,7 +5182,7 @@
         <v>366</v>
       </c>
       <c r="N48" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O48" s="1" t="s">
         <v>365</v>
@@ -5200,7 +5200,7 @@
         <v>317</v>
       </c>
       <c r="T48" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="49" spans="1:20" ht="202.8" x14ac:dyDescent="0.3">
@@ -5211,7 +5211,7 @@
         <v>295</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D49" s="11" t="s">
         <v>298</v>
@@ -5220,11 +5220,11 @@
         <v>318</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>40</v>
@@ -5250,12 +5250,14 @@
       <c r="Q49" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="R49" s="9"/>
+      <c r="R49" s="9" t="s">
+        <v>566</v>
+      </c>
       <c r="S49" s="9" t="s">
         <v>320</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="50" spans="1:20" ht="187.2" x14ac:dyDescent="0.3">
@@ -5266,7 +5268,7 @@
         <v>295</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>299</v>
@@ -5275,11 +5277,11 @@
         <v>321</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>40</v>
@@ -5291,13 +5293,13 @@
         <v>9</v>
       </c>
       <c r="L50" s="8" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="M50" s="8" t="s">
         <v>366</v>
       </c>
       <c r="N50" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O50" s="1" t="s">
         <v>365</v>
@@ -5315,7 +5317,7 @@
         <v>324</v>
       </c>
       <c r="T50" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="51" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -5326,7 +5328,7 @@
         <v>295</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>300</v>
@@ -5338,10 +5340,10 @@
         <v>326</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H51" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>40</v>
@@ -5359,7 +5361,7 @@
         <v>366</v>
       </c>
       <c r="N51" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>422</v>
@@ -5377,7 +5379,7 @@
         <v>329</v>
       </c>
       <c r="T51" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="52" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -5388,7 +5390,7 @@
         <v>295</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>301</v>
@@ -5397,13 +5399,13 @@
         <v>330</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H52" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>40</v>
@@ -5421,7 +5423,7 @@
         <v>366</v>
       </c>
       <c r="N52" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>435</v>
@@ -5439,7 +5441,7 @@
         <v>333</v>
       </c>
       <c r="T52" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="53" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -5450,7 +5452,7 @@
         <v>295</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>302</v>
@@ -5462,10 +5464,10 @@
         <v>335</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H53" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>40</v>
@@ -5483,7 +5485,7 @@
         <v>366</v>
       </c>
       <c r="N53" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>422</v>
@@ -5501,7 +5503,7 @@
         <v>338</v>
       </c>
       <c r="T53" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54" spans="1:20" ht="93.6" x14ac:dyDescent="0.3">
@@ -5512,7 +5514,7 @@
         <v>295</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>303</v>
@@ -5521,13 +5523,13 @@
         <v>339</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G54" s="8" t="s">
         <v>443</v>
       </c>
       <c r="H54" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>40</v>
@@ -5545,7 +5547,7 @@
         <v>366</v>
       </c>
       <c r="N54" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O54" s="1" t="s">
         <v>374</v>
@@ -5563,7 +5565,7 @@
         <v>342</v>
       </c>
       <c r="T54" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="55" spans="1:20" ht="124.8" x14ac:dyDescent="0.3">
@@ -5574,7 +5576,7 @@
         <v>295</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>304</v>
@@ -5587,7 +5589,7 @@
       </c>
       <c r="G55" s="8"/>
       <c r="H55" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>40</v>
@@ -5605,7 +5607,7 @@
         <v>366</v>
       </c>
       <c r="N55" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O55" s="1" t="s">
         <v>422</v>
@@ -5623,7 +5625,7 @@
         <v>347</v>
       </c>
       <c r="T55" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="56" spans="1:20" ht="109.2" x14ac:dyDescent="0.3">
@@ -5634,7 +5636,7 @@
         <v>295</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>305</v>
@@ -5643,11 +5645,11 @@
         <v>348</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G56" s="8"/>
       <c r="H56" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>40</v>
@@ -5665,7 +5667,7 @@
         <v>418</v>
       </c>
       <c r="N56" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O56" s="1" t="s">
         <v>438</v>
@@ -5683,7 +5685,7 @@
         <v>351</v>
       </c>
       <c r="T56" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="57" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -5694,7 +5696,7 @@
         <v>295</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>306</v>
@@ -5703,11 +5705,11 @@
         <v>352</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G57" s="8"/>
       <c r="H57" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>40</v>
@@ -5743,7 +5745,7 @@
         <v>354</v>
       </c>
       <c r="T57" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="58" spans="1:20" ht="140.4" x14ac:dyDescent="0.3">
@@ -5754,7 +5756,7 @@
         <v>295</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>307</v>
@@ -5763,11 +5765,11 @@
         <v>356</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G58" s="8"/>
       <c r="H58" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>40</v>
@@ -5779,13 +5781,13 @@
         <v>9</v>
       </c>
       <c r="L58" s="8" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M58" s="15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="N58" s="8" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O58" s="1" t="s">
         <v>440</v>
@@ -5803,7 +5805,7 @@
         <v>359</v>
       </c>
       <c r="T58" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="78" x14ac:dyDescent="0.3">
@@ -5814,7 +5816,7 @@
         <v>295</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>308</v>
@@ -5827,7 +5829,7 @@
       </c>
       <c r="G59" s="8"/>
       <c r="H59" s="8" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>40</v>
@@ -5845,7 +5847,7 @@
         <v>377</v>
       </c>
       <c r="N59" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="O59" s="1" t="s">
         <v>396</v>
@@ -5863,7 +5865,7 @@
         <v>363</v>
       </c>
       <c r="T59" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.3">
@@ -6341,10 +6343,11 @@
     <hyperlink ref="G42" r:id="rId168"/>
     <hyperlink ref="G44" r:id="rId169"/>
     <hyperlink ref="G52" r:id="rId170"/>
+    <hyperlink ref="R6" r:id="rId171"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId171"/>
-  <legacyDrawing r:id="rId172"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId172"/>
+  <legacyDrawing r:id="rId173"/>
 </worksheet>
 </file>
 

</xml_diff>